<commit_message>
status 2022 11 09
</commit_message>
<xml_diff>
--- a/Results/Results_quality_of_clusters/Other_Clustering/iris_Kmed_true_label_clust_eval.xlsx
+++ b/Results/Results_quality_of_clusters/Other_Clustering/iris_Kmed_true_label_clust_eval.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janez\Documents\MATLAB\jpcode\Exact_clustering_SOS_SDP\Results\Results_quality_of_clusters\Other_Clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E99225F4-971B-45D9-BD8C-A9480B96A1B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7C00FD-8784-4952-BD7F-8877D5F5E274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="7905"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11746" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -63,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,14 +420,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">

</xml_diff>